<commit_message>
get rid of aspectj from project fix logging for TextInput element
</commit_message>
<xml_diff>
--- a/AdminInputData.xlsx
+++ b/AdminInputData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>idTest</t>
   </si>
@@ -34,9 +34,6 @@
     <t>pass</t>
   </si>
   <si>
-    <t>Field</t>
-  </si>
-  <si>
     <t>ValidateLogin</t>
   </si>
   <si>
@@ -47,9 +44,6 @@
   </si>
   <si>
     <t>qwerty123</t>
-  </si>
-  <si>
-    <t>n/a</t>
   </si>
 </sst>
 </file>
@@ -195,20 +189,20 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="E1" activeCellId="0" sqref="E1:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.8348214285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2276785714286"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.84375"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.4285714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.5982142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.26785714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.4821428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9910714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.6071428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0714285714286"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.3616071428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.15178571428571"/>
   </cols>
   <sheetData>
-    <row r="1" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="3" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -221,11 +215,9 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="E1" s="2"/>
     </row>
-    <row r="2" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="3" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -238,26 +230,22 @@
       <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="B3" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="E3" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
add first test for catalogue management
</commit_message>
<xml_diff>
--- a/AdminInputData.xlsx
+++ b/AdminInputData.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="CatalogueManagement" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
   <si>
     <t>idTest</t>
   </si>
@@ -44,6 +45,9 @@
   </si>
   <si>
     <t>qwerty123</t>
+  </si>
+  <si>
+    <t>ViewCatalogueManagementPage</t>
   </si>
 </sst>
 </file>
@@ -186,20 +190,19 @@
   </sheetPr>
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E1" activeCellId="0" sqref="E1:E4"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.4821428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9910714285714"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.6071428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0714285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.3616071428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.15178571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.1294642857143"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.7589285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3705357142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.8348214285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.125"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -256,4 +259,77 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.6651785714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.9910714285714"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="3" customFormat="true" ht="16.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" s="3" customFormat="true" ht="16.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="5"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add kick off for second catalogues test
</commit_message>
<xml_diff>
--- a/AdminInputData.xlsx
+++ b/AdminInputData.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="19">
   <si>
     <t>idTest</t>
   </si>
@@ -47,7 +47,37 @@
     <t>qwerty123</t>
   </si>
   <si>
+    <t>shortName</t>
+  </si>
+  <si>
+    <t>longName</t>
+  </si>
+  <si>
+    <t>introDateDaysJump</t>
+  </si>
+  <si>
+    <t>exitDateDaysJump</t>
+  </si>
+  <si>
+    <t>configurationSet</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
     <t>ViewCatalogueManagementPage</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>AddNewCatalogue</t>
+  </si>
+  <si>
+    <t>auto_test_catalogue</t>
+  </si>
+  <si>
+    <t>auto_test_catalogue_please_ignore</t>
   </si>
 </sst>
 </file>
@@ -58,7 +88,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -95,6 +125,13 @@
       <name val="Century Gothic"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF000000"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -146,7 +183,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -168,6 +205,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -193,7 +234,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="1" sqref="I3:J3 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -266,16 +307,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.6651785714286"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.9910714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.9375"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6160714285714"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.2589285714286"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="16.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -291,7 +335,24 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" s="3" customFormat="true" ht="16.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -310,7 +371,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>5</v>
@@ -321,7 +382,44 @@
       <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="5"/>
+      <c r="E3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>